<commit_message>
Changed framework from .NET Framework 4.7.2 to .NET 7
</commit_message>
<xml_diff>
--- a/Documentation/CargoFlow_Gantt_UseCases.xlsx
+++ b/Documentation/CargoFlow_Gantt_UseCases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/19c2f1c6d7cf0253/Documents/T6 OneDrive/(Lu Me) Projet Prog - CargoFlow/CargoFlow Repo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/19c2f1c6d7cf0253/Documents/T6 OneDrive/(Lu Me) Projet Prog - CargoFlow/CargoFlow Repo/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{0C0CF97F-0183-47CE-9A98-397B9B4EDB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{577E5586-FEDB-4AAC-AD9C-62A4B65B7F25}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{AC07F81B-F181-4779-B2DE-D95D9C1702AF}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AC07F81B-F181-4779-B2DE-D95D9C1702AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="1" r:id="rId1"/>
@@ -551,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -589,12 +589,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -608,10 +606,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -619,7 +616,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
@@ -627,6 +623,12 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -635,12 +637,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -657,6 +653,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -958,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13446C14-564C-45DE-B22C-2144ABC83B63}">
   <dimension ref="B1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,22 +969,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41" t="s">
+      <c r="D1" s="39"/>
+      <c r="E1" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41" t="s">
+      <c r="F1" s="39"/>
+      <c r="G1" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41" t="s">
+      <c r="H1" s="39"/>
+      <c r="I1" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="41"/>
+      <c r="J1" s="39"/>
     </row>
     <row r="2" spans="2:11" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="6" t="s">
@@ -1019,211 +1019,211 @@
       <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="36"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="32"/>
     </row>
     <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="37"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="33"/>
     </row>
     <row r="5" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="37"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="33"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="37"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="33"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="37"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="33"/>
     </row>
     <row r="8" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="37"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="33"/>
     </row>
     <row r="9" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="37"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="33"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="37"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="33"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="37"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="33"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="37"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="33"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="37"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="33"/>
     </row>
     <row r="14" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="37"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="33"/>
     </row>
     <row r="15" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="37"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="33"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="37"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="33"/>
     </row>
     <row r="17" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="38"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1242,7 +1242,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{484903DD-0271-42B2-B1FE-55CB7C783076}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -1254,249 +1254,248 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="E1" s="13" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="E1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="36" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="16" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18" t="s">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="16" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="17" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="44"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-    </row>
-    <row r="6" spans="1:5" s="17" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
+    <row r="5" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="37"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+    </row>
+    <row r="6" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="38"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19" t="s">
+      <c r="B8" s="17"/>
+      <c r="C8" s="17" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="17" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
-      <c r="B10" s="19" t="s">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="17" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19" t="s">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="17" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="42" t="s">
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="42" t="s">
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="17"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="42"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="13"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="42" t="s">
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="17"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="19"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="19"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="17"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
+      <c r="A33" s="17"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="19"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
+      <c r="A34" s="17"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="19"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
+      <c r="A35" s="17"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
+      <c r="A36" s="17"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="19"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
+      <c r="A37" s="17"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="19"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
+      <c r="A38" s="17"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
+      <c r="A39" s="17"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1530,7 +1529,7 @@
     <col min="9" max="10" width="3.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="179.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="177.75" x14ac:dyDescent="0.25">
       <c r="B1" s="12" t="s">
         <v>29</v>
       </c>
@@ -1577,28 +1576,28 @@
       <c r="A3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="16"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1609,26 +1608,23 @@
       <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Create classes, update use cases
</commit_message>
<xml_diff>
--- a/Documentation/CargoFlow_Gantt_UseCases.xlsx
+++ b/Documentation/CargoFlow_Gantt_UseCases.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/19c2f1c6d7cf0253/Documents/T6 OneDrive/(Lu Me) Projet Prog - CargoFlow/CargoFlow Repo/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{0C0CF97F-0183-47CE-9A98-397B9B4EDB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{577E5586-FEDB-4AAC-AD9C-62A4B65B7F25}"/>
+  <xr:revisionPtr revIDLastSave="267" documentId="13_ncr:1_{0C0CF97F-0183-47CE-9A98-397B9B4EDB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CAFF421-F761-44FC-8F6C-389592A933BC}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AC07F81B-F181-4779-B2DE-D95D9C1702AF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{AC07F81B-F181-4779-B2DE-D95D9C1702AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="1" r:id="rId1"/>
-    <sheet name="Scénarios" sheetId="2" r:id="rId2"/>
+    <sheet name="Use cases" sheetId="4" r:id="rId2"/>
     <sheet name="Rôles" sheetId="3" r:id="rId3"/>
+    <sheet name="Rôles simplifiés" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="78">
   <si>
     <t>Initialisation</t>
   </si>
@@ -83,9 +84,6 @@
     <t>MCD/MLD</t>
   </si>
   <si>
-    <t>Ecrire tests</t>
-  </si>
-  <si>
     <t>Ecrire code métier</t>
   </si>
   <si>
@@ -149,63 +147,6 @@
     <t>Lire (consulter)</t>
   </si>
   <si>
-    <t>Vendeurs</t>
-  </si>
-  <si>
-    <t>Identification</t>
-  </si>
-  <si>
-    <t>L'utilisateur arrive sur sa page principale</t>
-  </si>
-  <si>
-    <t>Identification réussie</t>
-  </si>
-  <si>
-    <t>Chefs de la logistique</t>
-  </si>
-  <si>
-    <t>Gérants des entrepôts</t>
-  </si>
-  <si>
-    <t>Gérants des centres de production</t>
-  </si>
-  <si>
-    <t>Gérants des magasins</t>
-  </si>
-  <si>
-    <t>Une page présentant tous les centres de production, tous les entrepôts et tous les magasins.</t>
-  </si>
-  <si>
-    <t>Clic sur une entité</t>
-  </si>
-  <si>
-    <t>L'entité est un centre de production</t>
-  </si>
-  <si>
-    <t>L'entité est un entrepôt</t>
-  </si>
-  <si>
-    <t>Affichage du stock du centre de production avec possibilité de filtrer la liste</t>
-  </si>
-  <si>
-    <t>Affichage du stock de l'entrepôt avec possibilité de filtrer la liste</t>
-  </si>
-  <si>
-    <t>L'entité est magasin</t>
-  </si>
-  <si>
-    <t>Affichage du stock du magasin avec possibilité de filtrer la liste</t>
-  </si>
-  <si>
-    <t>L'user s'identifie correctement</t>
-  </si>
-  <si>
-    <t>L'user s'identifie mal</t>
-  </si>
-  <si>
-    <t>Un message d'erreur apparait</t>
-  </si>
-  <si>
     <t>Sprint 1</t>
   </si>
   <si>
@@ -215,22 +156,121 @@
     <t>Sprint 3</t>
   </si>
   <si>
-    <t>Tout ça peut être fait sprint par sprint, avec updates possibles</t>
-  </si>
-  <si>
-    <t>Use case 1 : En tant que user, je veux créer un compte et m'y connecter</t>
-  </si>
-  <si>
-    <t>Action (Given)</t>
-  </si>
-  <si>
-    <t>Condition (When)</t>
-  </si>
-  <si>
-    <t>Réaction (Then)</t>
-  </si>
-  <si>
     <t>Conception</t>
+  </si>
+  <si>
+    <t>En tant que chef de la logistique, je souhaite…</t>
+  </si>
+  <si>
+    <t>et les trier…</t>
+  </si>
+  <si>
+    <t>en même temps…</t>
+  </si>
+  <si>
+    <t>séparément…</t>
+  </si>
+  <si>
+    <t>et trier leurs articles…</t>
+  </si>
+  <si>
+    <t>et filtrer leurs articles…</t>
+  </si>
+  <si>
+    <t>En tant que gérant d'un entrepôt, je souhaite…</t>
+  </si>
+  <si>
+    <t>et trier ses articles…</t>
+  </si>
+  <si>
+    <t>et filtrer ses articles…</t>
+  </si>
+  <si>
+    <t>voir le prix total des articles contenus dans tous les entrepôts…</t>
+  </si>
+  <si>
+    <t>en même temps.</t>
+  </si>
+  <si>
+    <t>séparément.</t>
+  </si>
+  <si>
+    <t>par leur modèle.</t>
+  </si>
+  <si>
+    <t>par leur marque.</t>
+  </si>
+  <si>
+    <t>par leur id.</t>
+  </si>
+  <si>
+    <t>et voir les détails d'un article en cliquant dessus.</t>
+  </si>
+  <si>
+    <t>lister les employés des entrepôts et les entrepôts auxquels ils sont associés…</t>
+  </si>
+  <si>
+    <t>et voir les détails d'un employé en cliquant dessus.</t>
+  </si>
+  <si>
+    <t>par statut (en cours de livraison ou livré).</t>
+  </si>
+  <si>
+    <t>et voir les détails d'une livraison en cliquant dessus.</t>
+  </si>
+  <si>
+    <t>et voir les détails d'un transporteur en cliquant dessus.</t>
+  </si>
+  <si>
+    <t>et voir les détails d'un entrepôt en cliquant dessus.</t>
+  </si>
+  <si>
+    <t>lister les employés de mon entrepôt…</t>
+  </si>
+  <si>
+    <t>par commune de destination</t>
+  </si>
+  <si>
+    <t>lister tous les transporteurs…</t>
+  </si>
+  <si>
+    <t>lister tous les entrepôts…</t>
+  </si>
+  <si>
+    <t>lister tous les articles en stock de tous les entrepôts…</t>
+  </si>
+  <si>
+    <t>Gérant d'un entrepôt</t>
+  </si>
+  <si>
+    <t>Employé d'un entrepôt</t>
+  </si>
+  <si>
+    <t>lister tous les clients…</t>
+  </si>
+  <si>
+    <t>et voir les détails d'un client en cliquant dessus.</t>
+  </si>
+  <si>
+    <t>Maquettes Balsamiq</t>
+  </si>
+  <si>
+    <t>lister toutes les livraisons…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Liste des transporteurs</t>
+  </si>
+  <si>
+    <t>lister tous les articles en stock de mon entrepôt…</t>
+  </si>
+  <si>
+    <t>et voir les détails d'un transporteur en cliquant dessus…</t>
+  </si>
+  <si>
+    <t>et modifier les détails d'un transporteur si besoin.</t>
+  </si>
+  <si>
+    <t>et supprimer des transporteurs.</t>
   </si>
 </sst>
 </file>
@@ -335,13 +375,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -551,7 +591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -592,12 +632,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -620,22 +654,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -653,10 +676,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -958,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13446C14-564C-45DE-B22C-2144ABC83B63}">
   <dimension ref="B1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,22 +988,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39" t="s">
-        <v>58</v>
-      </c>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="J1" s="39"/>
+      <c r="C1" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="38"/>
     </row>
     <row r="2" spans="2:11" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="6" t="s">
@@ -1019,211 +1038,211 @@
       <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="32"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="30"/>
     </row>
     <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="33"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="31"/>
     </row>
     <row r="5" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="33"/>
+        <v>39</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="31"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="33"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="31"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="33"/>
-    </row>
-    <row r="8" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="31"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="33"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="31"/>
     </row>
     <row r="9" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="31"/>
+    </row>
+    <row r="10" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="33"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="33"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="31"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="33"/>
+        <v>21</v>
+      </c>
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="31"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="33"/>
+        <v>15</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="31"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="33"/>
+        <v>17</v>
+      </c>
+      <c r="C13" s="20"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="31"/>
     </row>
     <row r="14" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="33"/>
+        <v>20</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="31"/>
     </row>
     <row r="15" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="33"/>
+        <v>16</v>
+      </c>
+      <c r="C15" s="20"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="31"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="33"/>
+        <v>18</v>
+      </c>
+      <c r="C16" s="20"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="31"/>
     </row>
     <row r="17" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="34"/>
+        <v>19</v>
+      </c>
+      <c r="C17" s="24"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1239,273 +1258,323 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{484903DD-0271-42B2-B1FE-55CB7C783076}">
-  <dimension ref="A1:E39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0CEFB72-0386-4A3A-8E14-7FDFA075C118}">
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" customWidth="1"/>
+    <col min="1" max="1" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="35"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="35"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="35"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="35"/>
+      <c r="B7" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="35"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="35"/>
+      <c r="B9" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="35"/>
+      <c r="B10" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="36"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="35"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="36"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="35"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="35"/>
+      <c r="B13" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="35"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="35"/>
+      <c r="B15" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="35"/>
+      <c r="B16" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="34"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="34"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="34"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="34"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="34"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="34"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="34"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="34"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="34"/>
+      <c r="B22" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="34"/>
+      <c r="B23" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" s="34"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="34"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="34"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="34"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="34"/>
+      <c r="B26" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="34"/>
+      <c r="B27" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="E1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="34"/>
+      <c r="B28" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-    </row>
-    <row r="6" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="38"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
-    </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="40"/>
-      <c r="C22" s="40"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="40"/>
-      <c r="C27" s="40"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="17"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="17"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="17"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="17"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="17"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="17"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="17"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="17"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="17"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A22:C22"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1515,7 +1584,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1531,36 +1600,36 @@
   <sheetData>
     <row r="1" spans="1:10" ht="177.75" x14ac:dyDescent="0.25">
       <c r="B1" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>33</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -1574,7 +1643,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="14"/>
       <c r="C3" s="13"/>
@@ -1582,7 +1651,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="13"/>
@@ -1592,7 +1661,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="14"/>
       <c r="C5" s="13"/>
@@ -1601,12 +1670,12 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
@@ -1614,14 +1683,14 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
@@ -1630,4 +1699,92 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4CFAA94-5785-4B0B-9532-379E29F59DC0}">
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="11" width="4.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="139.5" x14ac:dyDescent="0.25">
+      <c r="B1" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Use Cases & wireframes
</commit_message>
<xml_diff>
--- a/Documentation/CargoFlow_Gantt_UseCases.xlsx
+++ b/Documentation/CargoFlow_Gantt_UseCases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/19c2f1c6d7cf0253/Documents/T6 OneDrive/(Lu Me) Projet Prog - CargoFlow/CargoFlow Repo/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cpnv\projProg\CargoFlow\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="476" documentId="13_ncr:1_{0C0CF97F-0183-47CE-9A98-397B9B4EDB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5840785F-11F2-45F8-ADD2-8BF9F75AA786}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8124FA-3359-4EA8-B769-0DB643AB18CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{AC07F81B-F181-4779-B2DE-D95D9C1702AF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{AC07F81B-F181-4779-B2DE-D95D9C1702AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="74">
   <si>
     <t>Initialisation</t>
   </si>
@@ -251,6 +251,12 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>par localité.</t>
+  </si>
+  <si>
+    <t>par NPA.</t>
   </si>
 </sst>
 </file>
@@ -612,9 +618,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -625,6 +628,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -641,10 +647,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -957,22 +959,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34" t="s">
+      <c r="D1" s="39"/>
+      <c r="E1" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34" t="s">
+      <c r="F1" s="39"/>
+      <c r="G1" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34" t="s">
+      <c r="H1" s="39"/>
+      <c r="I1" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="34"/>
+      <c r="J1" s="39"/>
     </row>
     <row r="2" spans="2:11" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="6" t="s">
@@ -1228,10 +1230,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0CEFB72-0386-4A3A-8E14-7FDFA075C118}">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1524,50 +1526,50 @@
         <v>39</v>
       </c>
       <c r="C29" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="E29" s="32"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="31"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="E30" s="32"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="31"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="30" t="s">
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B32" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="30" t="s">
+      <c r="C32" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="30" t="s">
+      <c r="D32" s="30" t="s">
         <v>33</v>
-      </c>
-      <c r="E30" s="30"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="E31" s="30"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30" t="s">
-        <v>31</v>
       </c>
       <c r="E32" s="30"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="30"/>
       <c r="B33" s="30"/>
-      <c r="C33" s="30" t="s">
-        <v>69</v>
-      </c>
+      <c r="C33" s="30"/>
       <c r="D33" s="30" t="s">
         <v>32</v>
       </c>
@@ -1585,79 +1587,77 @@
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="30"/>
       <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
+      <c r="C35" s="30" t="s">
+        <v>69</v>
+      </c>
       <c r="D35" s="30" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="E35" s="30"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="30"/>
-      <c r="B36" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="C36" s="33"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36" s="30"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="30"/>
-      <c r="B37" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="C37" s="30" t="s">
-        <v>69</v>
-      </c>
+      <c r="B37" s="30"/>
+      <c r="C37" s="30"/>
       <c r="D37" s="30" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E37" s="30"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="30"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="E38" s="30"/>
+      <c r="B38" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="33"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="33"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="30"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="30"/>
+      <c r="B39" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" s="30" t="s">
+        <v>69</v>
+      </c>
       <c r="D39" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E39" s="30"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="30"/>
       <c r="B40" s="30"/>
-      <c r="C40" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D40" s="30"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30" t="s">
+        <v>64</v>
+      </c>
       <c r="E40" s="30"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="30"/>
-      <c r="B41" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="C41" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="D41" s="33"/>
-      <c r="E41" s="33"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="E41" s="30"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="30"/>
-      <c r="B42" s="30" t="s">
-        <v>35</v>
-      </c>
+      <c r="B42" s="30"/>
       <c r="C42" s="30" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D42" s="30"/>
       <c r="E42" s="30"/>
@@ -1665,10 +1665,10 @@
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="30"/>
       <c r="B43" s="33" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="C43" s="33" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D43" s="33"/>
       <c r="E43" s="33"/>
@@ -1676,184 +1676,206 @@
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="30"/>
       <c r="B44" s="30" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C44" s="30" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D44" s="30"/>
       <c r="E44" s="30"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="30" t="s">
-        <v>71</v>
-      </c>
+      <c r="A45" s="30"/>
       <c r="B45" s="33" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C45" s="33" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D45" s="33"/>
       <c r="E45" s="33"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="35" t="s">
+      <c r="A46" s="30"/>
+      <c r="B46" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C47" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D47" s="33"/>
+      <c r="E47" s="33"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="B46" s="35" t="s">
+      <c r="B48" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="C46" s="35" t="s">
+      <c r="C48" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="D46" s="35" t="s">
+      <c r="D48" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="E46" s="35"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="39"/>
-      <c r="B47" s="35"/>
-      <c r="C47" s="35"/>
-      <c r="D47" s="35" t="s">
+      <c r="E48" s="34"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="38"/>
+      <c r="B49" s="34"/>
+      <c r="C49" s="34"/>
+      <c r="D49" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="E47" s="35"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="39"/>
-      <c r="B48" s="35"/>
-      <c r="C48" s="35"/>
-      <c r="D48" s="35" t="s">
+      <c r="E49" s="34"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="38"/>
+      <c r="B50" s="34"/>
+      <c r="C50" s="34"/>
+      <c r="D50" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="E48" s="35"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="39"/>
-      <c r="B49" s="35"/>
-      <c r="C49" s="35" t="s">
+      <c r="E50" s="34"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="38"/>
+      <c r="B51" s="34"/>
+      <c r="C51" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="D49" s="35" t="s">
+      <c r="D51" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="E49" s="35"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="39"/>
-      <c r="B50" s="35"/>
-      <c r="C50" s="35"/>
-      <c r="D50" s="35" t="s">
+      <c r="E51" s="34"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="38"/>
+      <c r="B52" s="34"/>
+      <c r="C52" s="34"/>
+      <c r="D52" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="E50" s="35"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="39"/>
-      <c r="B51" s="35"/>
-      <c r="C51" s="35"/>
-      <c r="D51" s="35" t="s">
+      <c r="E52" s="34"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="38"/>
+      <c r="B53" s="34"/>
+      <c r="C53" s="34"/>
+      <c r="D53" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="E51" s="35"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="39"/>
-      <c r="B52" s="36" t="s">
+      <c r="E53" s="34"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="38"/>
+      <c r="B54" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="C52" s="36"/>
-      <c r="D52" s="36"/>
-      <c r="E52" s="36"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="39"/>
-      <c r="B53" s="35" t="s">
+      <c r="C54" s="35"/>
+      <c r="D54" s="35"/>
+      <c r="E54" s="35"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="38"/>
+      <c r="B55" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="C53" s="35" t="s">
+      <c r="C55" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="D53" s="35" t="s">
+      <c r="D55" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="E53" s="35"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="39"/>
-      <c r="B54" s="35"/>
-      <c r="C54" s="35"/>
-      <c r="D54" s="35" t="s">
+      <c r="E55" s="34"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="38"/>
+      <c r="B56" s="34"/>
+      <c r="C56" s="34"/>
+      <c r="D56" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="E54" s="35"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="39"/>
-      <c r="B55" s="35"/>
-      <c r="C55" s="35"/>
-      <c r="D55" s="35" t="s">
+      <c r="E56" s="34"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="38"/>
+      <c r="B57" s="34"/>
+      <c r="C57" s="34"/>
+      <c r="D57" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="E55" s="35"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="39"/>
-      <c r="B56" s="35"/>
-      <c r="C56" s="35" t="s">
+      <c r="E57" s="34"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="38"/>
+      <c r="B58" s="34"/>
+      <c r="C58" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="D56" s="35"/>
-      <c r="E56" s="35"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="39"/>
-      <c r="B57" s="36" t="s">
+      <c r="D58" s="34"/>
+      <c r="E58" s="34"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="38"/>
+      <c r="B59" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="C57" s="36" t="s">
+      <c r="C59" s="35" t="s">
         <v>44</v>
-      </c>
-      <c r="D57" s="36"/>
-      <c r="E57" s="36"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="39"/>
-      <c r="B58" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="C58" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="D58" s="35"/>
-      <c r="E58" s="35"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="37"/>
-      <c r="B59" s="35"/>
-      <c r="C59" s="35" t="s">
-        <v>67</v>
       </c>
       <c r="D59" s="35"/>
       <c r="E59" s="35"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="37"/>
-      <c r="B60" s="35"/>
-      <c r="C60" s="35" t="s">
+      <c r="A60" s="38"/>
+      <c r="B60" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C60" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="D60" s="34"/>
+      <c r="E60" s="34"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="36"/>
+      <c r="B61" s="34"/>
+      <c r="C61" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="D61" s="34"/>
+      <c r="E61" s="34"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="36"/>
+      <c r="B62" s="34"/>
+      <c r="C62" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="D60" s="35"/>
-      <c r="E60" s="35"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="38"/>
-      <c r="B62" s="38"/>
-      <c r="C62" s="38"/>
-      <c r="D62" s="38"/>
-      <c r="E62" s="38"/>
+      <c r="D62" s="34"/>
+      <c r="E62" s="34"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="37"/>
+      <c r="B64" s="37"/>
+      <c r="C64" s="37"/>
+      <c r="D64" s="37"/>
+      <c r="E64" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update wireframe + use cases
</commit_message>
<xml_diff>
--- a/Documentation/CargoFlow_Gantt_UseCases.xlsx
+++ b/Documentation/CargoFlow_Gantt_UseCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cpnv\projProg\CargoFlow\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8124FA-3359-4EA8-B769-0DB643AB18CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C948CC-B9E0-4459-ADE9-137E4F0FCF09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{AC07F81B-F181-4779-B2DE-D95D9C1702AF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="80">
   <si>
     <t>Initialisation</t>
   </si>
@@ -257,6 +257,24 @@
   </si>
   <si>
     <t>par NPA.</t>
+  </si>
+  <si>
+    <t>par leur nom.</t>
+  </si>
+  <si>
+    <t>par leur titre.</t>
+  </si>
+  <si>
+    <t>par leur poids.</t>
+  </si>
+  <si>
+    <t>lister le stock de tous les entrepôts…</t>
+  </si>
+  <si>
+    <t>lister les articles existants…</t>
+  </si>
+  <si>
+    <t>par leur catégorie.</t>
   </si>
 </sst>
 </file>
@@ -1230,10 +1248,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0CEFB72-0386-4A3A-8E14-7FDFA075C118}">
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,7 +1269,7 @@
         <v>26</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="C1" s="31" t="s">
         <v>27</v>
@@ -1286,7 +1304,7 @@
         <v>69</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="E4" s="31"/>
     </row>
@@ -1295,29 +1313,29 @@
       <c r="B5" s="31"/>
       <c r="C5" s="31"/>
       <c r="D5" s="31" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="E5" s="31"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="31"/>
+      <c r="B6" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="32"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="31"/>
-      <c r="B7" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>69</v>
-      </c>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
       <c r="D7" s="32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E7" s="32"/>
     </row>
@@ -1326,56 +1344,54 @@
       <c r="B8" s="32"/>
       <c r="C8" s="32"/>
       <c r="D8" s="32" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E8" s="32"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="31"/>
       <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32" t="s">
-        <v>66</v>
-      </c>
+      <c r="C9" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="32"/>
       <c r="E9" s="32"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="31"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
+      <c r="B10" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="31"/>
-      <c r="B11" s="31" t="s">
-        <v>29</v>
-      </c>
+      <c r="B11" s="31"/>
       <c r="C11" s="31" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="D11" s="31"/>
       <c r="E11" s="31"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
+      <c r="B12" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="31"/>
-      <c r="B13" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="32" t="s">
-        <v>44</v>
-      </c>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
       <c r="D13" s="32"/>
       <c r="E13" s="32"/>
     </row>
@@ -1383,264 +1399,266 @@
       <c r="A14" s="31"/>
       <c r="B14" s="32"/>
       <c r="C14" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="32"/>
+        <v>69</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>32</v>
+      </c>
       <c r="E14" s="32"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="31"/>
       <c r="B15" s="32"/>
-      <c r="C15" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32" t="s">
+        <v>76</v>
+      </c>
       <c r="E15" s="32"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="31"/>
       <c r="B16" s="32"/>
       <c r="C16" s="32" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="D16" s="32"/>
       <c r="E16" s="32"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="31"/>
-      <c r="B17" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="31"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="31"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="31"/>
-      <c r="B20" s="31"/>
+      <c r="B20" s="31" t="s">
+        <v>34</v>
+      </c>
       <c r="C20" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" s="31"/>
+        <v>69</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>75</v>
+      </c>
       <c r="E20" s="31"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="31"/>
-      <c r="B21" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="31"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="31"/>
-      <c r="B23" s="32"/>
-      <c r="C23" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="31"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="31"/>
-      <c r="B25" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
+      <c r="B25" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" s="32"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="31"/>
-      <c r="B26" s="31"/>
-      <c r="C26" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="31"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="31"/>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="31"/>
-      <c r="B29" s="32" t="s">
-        <v>39</v>
-      </c>
+      <c r="B29" s="32"/>
       <c r="C29" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="D29" s="32" t="s">
-        <v>72</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D29" s="32"/>
       <c r="E29" s="32"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="31"/>
-      <c r="B30" s="32"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="E30" s="32"/>
+      <c r="B30" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="31"/>
-      <c r="B31" s="32"/>
-      <c r="C31" s="32" t="s">
+      <c r="B31" s="31"/>
+      <c r="C31" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="31"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="31"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="31"/>
+      <c r="B34" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="E34" s="32"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="31"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" s="32"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="31"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="30" t="s">
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="30" t="s">
+      <c r="B37" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="30" t="s">
+      <c r="C37" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D32" s="30" t="s">
+      <c r="D37" s="30" t="s">
         <v>33</v>
-      </c>
-      <c r="E32" s="30"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="E33" s="30"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="E34" s="30"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="D35" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="E35" s="30"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="30"/>
-      <c r="B36" s="30"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="E36" s="30"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="30"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30" t="s">
-        <v>70</v>
       </c>
       <c r="E37" s="30"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="30"/>
-      <c r="B38" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="C38" s="33"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
+      <c r="B38" s="30"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="E38" s="30"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="30"/>
-      <c r="B39" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="C39" s="30" t="s">
-        <v>69</v>
-      </c>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
       <c r="D39" s="30" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="E39" s="30"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="30"/>
       <c r="B40" s="30"/>
-      <c r="C40" s="30"/>
+      <c r="C40" s="30" t="s">
+        <v>69</v>
+      </c>
       <c r="D40" s="30" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="E40" s="30"/>
     </row>
@@ -1649,166 +1667,166 @@
       <c r="B41" s="30"/>
       <c r="C41" s="30"/>
       <c r="D41" s="30" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="E41" s="30"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="30"/>
       <c r="B42" s="30"/>
-      <c r="C42" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D42" s="30"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="30" t="s">
+        <v>70</v>
+      </c>
       <c r="E42" s="30"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="30"/>
       <c r="B43" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="C43" s="33" t="s">
-        <v>44</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="C43" s="33"/>
       <c r="D43" s="33"/>
       <c r="E43" s="33"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="30"/>
       <c r="B44" s="30" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C44" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="D44" s="30"/>
+        <v>69</v>
+      </c>
+      <c r="D44" s="30" t="s">
+        <v>65</v>
+      </c>
       <c r="E44" s="30"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="30"/>
-      <c r="B45" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="C45" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="D45" s="33"/>
-      <c r="E45" s="33"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E45" s="30"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="30"/>
-      <c r="B46" s="30" t="s">
+      <c r="B46" s="30"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="E46" s="30"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="30"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D47" s="30"/>
+      <c r="E47" s="30"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="30"/>
+      <c r="B48" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D48" s="33"/>
+      <c r="E48" s="33"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="30"/>
+      <c r="B49" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C49" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="D49" s="30"/>
+      <c r="E49" s="30"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="30"/>
+      <c r="B50" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C50" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="D50" s="33"/>
+      <c r="E50" s="33"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="30"/>
+      <c r="B51" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="C46" s="30" t="s">
+      <c r="C51" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D46" s="30"/>
-      <c r="E46" s="30"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="30" t="s">
+      <c r="D51" s="30"/>
+      <c r="E51" s="30"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="B47" s="33" t="s">
+      <c r="B52" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C47" s="33" t="s">
+      <c r="C52" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="D47" s="33"/>
-      <c r="E47" s="33"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="34" t="s">
+      <c r="D52" s="33"/>
+      <c r="E52" s="33"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="B48" s="34" t="s">
+      <c r="B53" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="34" t="s">
+      <c r="C53" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="D48" s="34" t="s">
+      <c r="D53" s="34" t="s">
         <v>33</v>
-      </c>
-      <c r="E48" s="34"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="38"/>
-      <c r="B49" s="34"/>
-      <c r="C49" s="34"/>
-      <c r="D49" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="E49" s="34"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="38"/>
-      <c r="B50" s="34"/>
-      <c r="C50" s="34"/>
-      <c r="D50" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="E50" s="34"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="38"/>
-      <c r="B51" s="34"/>
-      <c r="C51" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="D51" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="E51" s="34"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="38"/>
-      <c r="B52" s="34"/>
-      <c r="C52" s="34"/>
-      <c r="D52" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="E52" s="34"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="38"/>
-      <c r="B53" s="34"/>
-      <c r="C53" s="34"/>
-      <c r="D53" s="34" t="s">
-        <v>70</v>
       </c>
       <c r="E53" s="34"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="38"/>
-      <c r="B54" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="C54" s="35"/>
-      <c r="D54" s="35"/>
-      <c r="E54" s="35"/>
+      <c r="B54" s="34"/>
+      <c r="C54" s="34"/>
+      <c r="D54" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E54" s="34"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="38"/>
-      <c r="B55" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="C55" s="34" t="s">
-        <v>69</v>
-      </c>
+      <c r="B55" s="34"/>
+      <c r="C55" s="34"/>
       <c r="D55" s="34" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="E55" s="34"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="38"/>
       <c r="B56" s="34"/>
-      <c r="C56" s="34"/>
+      <c r="C56" s="34" t="s">
+        <v>69</v>
+      </c>
       <c r="D56" s="34" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="E56" s="34"/>
     </row>
@@ -1817,65 +1835,114 @@
       <c r="B57" s="34"/>
       <c r="C57" s="34"/>
       <c r="D57" s="34" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="E57" s="34"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="38"/>
       <c r="B58" s="34"/>
-      <c r="C58" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="D58" s="34"/>
+      <c r="C58" s="34"/>
+      <c r="D58" s="34" t="s">
+        <v>70</v>
+      </c>
       <c r="E58" s="34"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="38"/>
       <c r="B59" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="C59" s="35" t="s">
-        <v>44</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="C59" s="35"/>
       <c r="D59" s="35"/>
       <c r="E59" s="35"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="38"/>
       <c r="B60" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C60" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="D60" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="E60" s="34"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="38"/>
+      <c r="B61" s="34"/>
+      <c r="C61" s="34"/>
+      <c r="D61" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="E61" s="34"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="38"/>
+      <c r="B62" s="34"/>
+      <c r="C62" s="34"/>
+      <c r="D62" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="E62" s="34"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="38"/>
+      <c r="B63" s="34"/>
+      <c r="C63" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D63" s="34"/>
+      <c r="E63" s="34"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="38"/>
+      <c r="B64" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C64" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="D64" s="35"/>
+      <c r="E64" s="35"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="38"/>
+      <c r="B65" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C60" s="34" t="s">
+      <c r="C65" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="D60" s="34"/>
-      <c r="E60" s="34"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="36"/>
-      <c r="B61" s="34"/>
-      <c r="C61" s="34" t="s">
+      <c r="D65" s="34"/>
+      <c r="E65" s="34"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="36"/>
+      <c r="B66" s="34"/>
+      <c r="C66" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="D61" s="34"/>
-      <c r="E61" s="34"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="36"/>
-      <c r="B62" s="34"/>
-      <c r="C62" s="34" t="s">
+      <c r="D66" s="34"/>
+      <c r="E66" s="34"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="36"/>
+      <c r="B67" s="34"/>
+      <c r="C67" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="D62" s="34"/>
-      <c r="E62" s="34"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="37"/>
-      <c r="B64" s="37"/>
-      <c r="C64" s="37"/>
-      <c r="D64" s="37"/>
-      <c r="E64" s="37"/>
+      <c r="D67" s="34"/>
+      <c r="E67" s="34"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="37"/>
+      <c r="B69" s="37"/>
+      <c r="C69" s="37"/>
+      <c r="D69" s="37"/>
+      <c r="E69" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FrmLists : Get column name when clicking on column header
</commit_message>
<xml_diff>
--- a/Documentation/CargoFlow_Gantt_UseCases.xlsx
+++ b/Documentation/CargoFlow_Gantt_UseCases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cpnv\projProg\CargoFlow\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/19c2f1c6d7cf0253/Documents/T6 OneDrive/(Lu Me) Projet Prog - CargoFlow/CargoFlow Repo/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C948CC-B9E0-4459-ADE9-137E4F0FCF09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{90C948CC-B9E0-4459-ADE9-137E4F0FCF09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A4788DD-46DA-4C47-84EA-226B86FD7237}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{AC07F81B-F181-4779-B2DE-D95D9C1702AF}"/>
+    <workbookView minimized="1" xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{AC07F81B-F181-4779-B2DE-D95D9C1702AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="1" r:id="rId1"/>
@@ -1251,7 +1251,7 @@
   <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>